<commit_message>
Gives realistic-looking values now
Matches the Reference 8 NASA data reasonably-well ish now
</commit_message>
<xml_diff>
--- a/NQLDW019 Problem BA.xlsx
+++ b/NQLDW019 Problem BA.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/dug20_cam_ac_uk/Documents/Cambridge/CUSF/6DOF-Trajectory-Simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{61603DC5-A56D-4A40-BE11-46A8A31BD09A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{61F5CE13-90C6-4D98-B683-294B3C12D96E}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{61603DC5-A56D-4A40-BE11-46A8A31BD09A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34CF3C71-BDF0-4A8E-A9B7-A629FD4A9DCF}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{F50538C7-0EDC-4A72-B785-78737CC82F01}"/>
   </bookViews>
   <sheets>
     <sheet name="Stagnation Point" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1082,4 +1083,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABC20A9-C40E-439F-9426-576600873B26}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>